<commit_message>
AFTA Selenium to Katalon Project
</commit_message>
<xml_diff>
--- a/Imp Files/ExportExcel.xlsx
+++ b/Imp Files/ExportExcel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t xml:space="preserve">S.No</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t>ppassdadf</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>saraswathi</t>
+  </si>
+  <si>
+    <t>fjhgkkl</t>
   </si>
 </sst>
 </file>
@@ -200,13 +209,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048572"/>

</xml_diff>

<commit_message>
Read and Write operations
</commit_message>
<xml_diff>
--- a/Imp Files/ExportExcel.xlsx
+++ b/Imp Files/ExportExcel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="22">
   <si>
     <t xml:space="preserve">S.No</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>fjhgkkl</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>raja</t>
+  </si>
+  <si>
+    <t>atchuta apartment</t>
+  </si>
+  <si>
+    <t>encryptedpass</t>
   </si>
 </sst>
 </file>
@@ -209,13 +221,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048572"/>

</xml_diff>